<commit_message>
fix: renamed sheet names for working with test_regression_core.py
</commit_message>
<xml_diff>
--- a/tests/regression_test_data.xlsx
+++ b/tests/regression_test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MLR\interactive-stepwise-regression-ui\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26EB5C71-3FFA-49FD-AE85-4FB710C7B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368AB46E-E691-488B-A5A7-D3BB3CE2D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Уравнение регрессии" sheetId="1" r:id="rId1"/>
-    <sheet name="Проверка через функции Excel" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Расчет" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -893,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2561,11 +2561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="O73" sqref="O73"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2629,7 +2632,7 @@
         <v>26.035063222603359</v>
       </c>
       <c r="O2">
-        <f>L2-N2</f>
+        <f t="shared" ref="O2:O27" si="0">L2-N2</f>
         <v>-3.2226033575000201E-6</v>
       </c>
       <c r="P2">
@@ -2637,7 +2640,7 @@
         <v>40.511308668046361</v>
       </c>
       <c r="Q2" s="25">
-        <f>ABS(O2)/L2</f>
+        <f t="shared" ref="Q2:Q27" si="1">ABS(O2)/L2</f>
         <v>1.2377937125937179E-7</v>
       </c>
     </row>
@@ -2683,7 +2686,7 @@
         <v>38.740628996626413</v>
       </c>
       <c r="O3">
-        <f>L3-N3</f>
+        <f t="shared" si="0"/>
         <v>1.0033735904357854E-6</v>
       </c>
       <c r="P3">
@@ -2691,7 +2694,7 @@
         <v>40.204736946868088</v>
       </c>
       <c r="Q3" s="25">
-        <f>ABS(O3)/L3</f>
+        <f t="shared" si="1"/>
         <v>2.5899774743874463E-8</v>
       </c>
     </row>
@@ -2737,7 +2740,7 @@
         <v>35.015823189882809</v>
       </c>
       <c r="O4">
-        <f>L4-N4</f>
+        <f t="shared" si="0"/>
         <v>6.8101171919465742E-6</v>
       </c>
       <c r="P4">
@@ -2745,7 +2748,7 @@
         <v>6.8430402635449381</v>
       </c>
       <c r="Q4" s="25">
-        <f>ABS(O4)/L4</f>
+        <f t="shared" si="1"/>
         <v>1.9448681330548423E-7</v>
       </c>
     </row>
@@ -2791,7 +2794,7 @@
         <v>38.855958684175874</v>
       </c>
       <c r="O5">
-        <f>L5-N5</f>
+        <f t="shared" si="0"/>
         <v>-8.684175874407174E-6</v>
       </c>
       <c r="P5">
@@ -2799,7 +2802,7 @@
         <v>41.680459434258815</v>
       </c>
       <c r="Q5" s="25">
-        <f>ABS(O5)/L5</f>
+        <f t="shared" si="1"/>
         <v>2.2349668131668827E-7</v>
       </c>
     </row>
@@ -2845,7 +2848,7 @@
         <v>38.52621298616311</v>
       </c>
       <c r="O6">
-        <f>L6-N6</f>
+        <f t="shared" si="0"/>
         <v>-2.9861631105632114E-6</v>
       </c>
       <c r="P6">
@@ -2853,7 +2856,7 @@
         <v>37.531558287554184</v>
       </c>
       <c r="Q6" s="25">
-        <f>ABS(O6)/L6</f>
+        <f t="shared" si="1"/>
         <v>7.7509911059593233E-8</v>
       </c>
     </row>
@@ -2899,7 +2902,7 @@
         <v>45.30356185119107</v>
       </c>
       <c r="O7">
-        <f>L7-N7</f>
+        <f t="shared" si="0"/>
         <v>8.1488089307413247E-6</v>
       </c>
       <c r="P7">
@@ -2907,7 +2910,7 @@
         <v>166.50445529184967</v>
       </c>
       <c r="Q7" s="25">
-        <f>ABS(O7)/L7</f>
+        <f t="shared" si="1"/>
         <v>1.7987123157714337E-7</v>
       </c>
     </row>
@@ -2953,7 +2956,7 @@
         <v>9.189302470419408</v>
       </c>
       <c r="O8">
-        <f>L8-N8</f>
+        <f t="shared" si="0"/>
         <v>4.5295805914946641E-6</v>
       </c>
       <c r="P8">
@@ -2961,7 +2964,7 @@
         <v>538.73206662757502</v>
       </c>
       <c r="Q8" s="25">
-        <f>ABS(O8)/L8</f>
+        <f t="shared" si="1"/>
         <v>4.9291862721472517E-7</v>
       </c>
     </row>
@@ -3007,7 +3010,7 @@
         <v>19.326641046455386</v>
       </c>
       <c r="O9">
-        <f>L9-N9</f>
+        <f t="shared" si="0"/>
         <v>-1.0464553845679347E-6</v>
       </c>
       <c r="P9">
@@ -3015,7 +3018,7 @@
         <v>170.91037441399396</v>
       </c>
       <c r="Q9" s="25">
-        <f>ABS(O9)/L9</f>
+        <f t="shared" si="1"/>
         <v>5.414574828153961E-8</v>
       </c>
     </row>
@@ -3061,7 +3064,7 @@
         <v>5.2532796663087629</v>
       </c>
       <c r="O10">
-        <f>L10-N10</f>
+        <f t="shared" si="0"/>
         <v>-6.6630876283113594E-7</v>
       </c>
       <c r="P10">
@@ -3069,7 +3072,7 @@
         <v>736.93954541532764</v>
       </c>
       <c r="Q10" s="25">
-        <f>ABS(O10)/L10</f>
+        <f t="shared" si="1"/>
         <v>1.2683673622343986E-7</v>
       </c>
     </row>
@@ -3115,7 +3118,7 @@
         <v>48.186951948272039</v>
       </c>
       <c r="O11">
-        <f>L11-N11</f>
+        <f t="shared" si="0"/>
         <v>-1.1948272039319363E-5</v>
       </c>
       <c r="P11">
@@ -3123,7 +3126,7 @@
         <v>249.23033322231737</v>
       </c>
       <c r="Q11" s="25">
-        <f>ABS(O11)/L11</f>
+        <f t="shared" si="1"/>
         <v>2.4795664633029951E-7</v>
       </c>
     </row>
@@ -3169,7 +3172,7 @@
         <v>27.136089644373062</v>
       </c>
       <c r="O12">
-        <f>L12-N12</f>
+        <f t="shared" si="0"/>
         <v>3.5562693767587916E-7</v>
       </c>
       <c r="P12">
@@ -3177,7 +3180,7 @@
         <v>27.707795323671011</v>
       </c>
       <c r="Q12" s="25">
-        <f>ABS(O12)/L12</f>
+        <f t="shared" si="1"/>
         <v>1.3105312433584912E-8</v>
       </c>
     </row>
@@ -3223,7 +3226,7 @@
         <v>50.595179579233545</v>
       </c>
       <c r="O13">
-        <f>L13-N13</f>
+        <f t="shared" si="0"/>
         <v>1.0420766457741593E-5</v>
       </c>
       <c r="P13">
@@ -3231,7 +3234,7 @@
         <v>331.06823387331747</v>
       </c>
       <c r="Q13" s="25">
-        <f>ABS(O13)/L13</f>
+        <f t="shared" si="1"/>
         <v>2.0596357989250741E-7</v>
       </c>
     </row>
@@ -3277,7 +3280,7 @@
         <v>45.222133144687149</v>
       </c>
       <c r="O14">
-        <f>L14-N14</f>
+        <f t="shared" si="0"/>
         <v>-3.1446871489038131E-6</v>
       </c>
       <c r="P14">
@@ -3285,7 +3288,7 @@
         <v>164.40933953694503</v>
       </c>
       <c r="Q14" s="25">
-        <f>ABS(O14)/L14</f>
+        <f t="shared" si="1"/>
         <v>6.9538678273310276E-8</v>
       </c>
     </row>
@@ -3331,7 +3334,7 @@
         <v>39.26274362009822</v>
       </c>
       <c r="O15">
-        <f>L15-N15</f>
+        <f t="shared" si="0"/>
         <v>6.379901776654151E-6</v>
       </c>
       <c r="P15">
@@ -3339,7 +3342,7 @@
         <v>47.098580256351084</v>
       </c>
       <c r="Q15" s="25">
-        <f>ABS(O15)/L15</f>
+        <f t="shared" si="1"/>
         <v>1.6249248401230559E-7</v>
       </c>
     </row>
@@ -3385,7 +3388,7 @@
         <v>14.653320024317317</v>
       </c>
       <c r="O16">
-        <f>L16-N16</f>
+        <f t="shared" si="0"/>
         <v>-2.431731616070465E-8</v>
       </c>
       <c r="P16">
@@ -3393,7 +3396,7 @@
         <v>314.94143751638779</v>
       </c>
       <c r="Q16" s="25">
-        <f>ABS(O16)/L16</f>
+        <f t="shared" si="1"/>
         <v>1.659508982312858E-9</v>
       </c>
     </row>
@@ -3439,7 +3442,7 @@
         <v>44.948480407189621</v>
       </c>
       <c r="O17">
-        <f>L17-N17</f>
+        <f t="shared" si="0"/>
         <v>-4.0718961713537283E-7</v>
       </c>
       <c r="P17">
@@ -3447,7 +3450,7 @@
         <v>157.46662255874512</v>
       </c>
       <c r="Q17" s="25">
-        <f>ABS(O17)/L17</f>
+        <f t="shared" si="1"/>
         <v>9.0590297410584925E-9</v>
       </c>
     </row>
@@ -3493,7 +3496,7 @@
         <v>32.25681720066104</v>
       </c>
       <c r="O18">
-        <f>L18-N18</f>
+        <f t="shared" si="0"/>
         <v>2.7993389579705763E-6</v>
       </c>
       <c r="P18">
@@ -3501,7 +3504,7 @@
         <v>2.047459400336608E-2</v>
       </c>
       <c r="Q18" s="25">
-        <f>ABS(O18)/L18</f>
+        <f t="shared" si="1"/>
         <v>8.6782855779663845E-8</v>
       </c>
     </row>
@@ -3547,7 +3550,7 @@
         <v>37.781020410530871</v>
       </c>
       <c r="O19">
-        <f>L19-N19</f>
+        <f t="shared" si="0"/>
         <v>-4.1053087329601112E-7</v>
       </c>
       <c r="P19">
@@ -3555,7 +3558,7 @@
         <v>28.956350627141862</v>
       </c>
       <c r="Q19" s="25">
-        <f>ABS(O19)/L19</f>
+        <f t="shared" si="1"/>
         <v>1.0866061141176473E-8</v>
       </c>
     </row>
@@ -3601,7 +3604,7 @@
         <v>21.168820559425473</v>
       </c>
       <c r="O20">
-        <f>L20-N20</f>
+        <f t="shared" si="0"/>
         <v>-5.5942547305676271E-7</v>
       </c>
       <c r="P20">
@@ -3609,7 +3612,7 @@
         <v>126.13737049308017</v>
       </c>
       <c r="Q20" s="25">
-        <f>ABS(O20)/L20</f>
+        <f t="shared" si="1"/>
         <v>2.6426861443234091E-8</v>
       </c>
     </row>
@@ -3655,7 +3658,7 @@
         <v>25.635152711607429</v>
       </c>
       <c r="O21">
-        <f>L21-N21</f>
+        <f t="shared" si="0"/>
         <v>-2.7116074292621306E-6</v>
       </c>
       <c r="P21">
@@ -3663,7 +3666,7 @@
         <v>45.761970572474077</v>
       </c>
       <c r="Q21" s="25">
-        <f>ABS(O21)/L21</f>
+        <f t="shared" si="1"/>
         <v>1.0577692852439446E-7</v>
       </c>
     </row>
@@ -3709,7 +3712,7 @@
         <v>40.422562462533605</v>
       </c>
       <c r="O22">
-        <f>L22-N22</f>
+        <f t="shared" si="0"/>
         <v>7.537466395035608E-6</v>
       </c>
       <c r="P22">
@@ -3717,7 +3720,7 @@
         <v>64.363082115388067</v>
       </c>
       <c r="Q22" s="25">
-        <f>ABS(O22)/L22</f>
+        <f t="shared" si="1"/>
         <v>1.8646677821414146E-7</v>
       </c>
     </row>
@@ -3763,7 +3766,7 @@
         <v>15.246817161811412</v>
       </c>
       <c r="O23">
-        <f>L23-N23</f>
+        <f t="shared" si="0"/>
         <v>2.838188587261925E-6</v>
       </c>
       <c r="P23">
@@ -3771,7 +3774,7 @@
         <v>294.22847807554166</v>
       </c>
       <c r="Q23" s="25">
-        <f>ABS(O23)/L23</f>
+        <f t="shared" si="1"/>
         <v>1.8614954379089705E-7</v>
       </c>
     </row>
@@ -3817,7 +3820,7 @@
         <v>28.678232870435906</v>
       </c>
       <c r="O24">
-        <f>L24-N24</f>
+        <f t="shared" si="0"/>
         <v>-2.8704359067432961E-6</v>
       </c>
       <c r="P24">
@@ -3825,7 +3828,7 @@
         <v>13.850898014437181</v>
       </c>
       <c r="Q24" s="25">
-        <f>ABS(O24)/L24</f>
+        <f t="shared" si="1"/>
         <v>1.0009111115795138E-7</v>
       </c>
     </row>
@@ -3871,7 +3874,7 @@
         <v>48.141080049067014</v>
       </c>
       <c r="O25">
-        <f>L25-N25</f>
+        <f t="shared" si="0"/>
         <v>-4.9067011786974035E-8</v>
       </c>
       <c r="P25">
@@ -3879,7 +3882,7 @@
         <v>247.78444992092975</v>
       </c>
       <c r="Q25" s="25">
-        <f>ABS(O25)/L25</f>
+        <f t="shared" si="1"/>
         <v>1.0192337144695141E-9</v>
       </c>
     </row>
@@ -3925,7 +3928,7 @@
         <v>40.147488385176963</v>
       </c>
       <c r="O26">
-        <f>L26-N26</f>
+        <f t="shared" si="0"/>
         <v>-8.3851769616671845E-6</v>
       </c>
       <c r="P26">
@@ -3933,7 +3936,7 @@
         <v>60.02484924843732</v>
       </c>
       <c r="Q26" s="25">
-        <f>ABS(O26)/L26</f>
+        <f t="shared" si="1"/>
         <v>2.0885935958289746E-7</v>
       </c>
     </row>
@@ -3979,7 +3982,7 @@
         <v>26.668283706736183</v>
       </c>
       <c r="O27">
-        <f>L27-N27</f>
+        <f t="shared" si="0"/>
         <v>-3.7067361837728185E-6</v>
       </c>
       <c r="P27">
@@ -3987,7 +3990,7 @@
         <v>32.851576284375625</v>
       </c>
       <c r="Q27" s="25">
-        <f>ABS(O27)/L27</f>
+        <f t="shared" si="1"/>
         <v>1.3899419774251727E-7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Regression core test corrections (#2)
* fix: сorrection of errors in the code, adjustment of relative error values (rtol)

* fix: renamed sheet names for working with test_regression_core.py

* fix: corrections to PAC and FSKF formulas

---------

Co-authored-by: suaviludius <powerranger1912@gmail.com.com>
</commit_message>
<xml_diff>
--- a/tests/regression_test_data.xlsx
+++ b/tests/regression_test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MLR\interactive-stepwise-regression-ui\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26EB5C71-3FFA-49FD-AE85-4FB710C7B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368AB46E-E691-488B-A5A7-D3BB3CE2D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Уравнение регрессии" sheetId="1" r:id="rId1"/>
-    <sheet name="Проверка через функции Excel" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Расчет" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -893,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2561,11 +2561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="O73" sqref="O73"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2629,7 +2632,7 @@
         <v>26.035063222603359</v>
       </c>
       <c r="O2">
-        <f>L2-N2</f>
+        <f t="shared" ref="O2:O27" si="0">L2-N2</f>
         <v>-3.2226033575000201E-6</v>
       </c>
       <c r="P2">
@@ -2637,7 +2640,7 @@
         <v>40.511308668046361</v>
       </c>
       <c r="Q2" s="25">
-        <f>ABS(O2)/L2</f>
+        <f t="shared" ref="Q2:Q27" si="1">ABS(O2)/L2</f>
         <v>1.2377937125937179E-7</v>
       </c>
     </row>
@@ -2683,7 +2686,7 @@
         <v>38.740628996626413</v>
       </c>
       <c r="O3">
-        <f>L3-N3</f>
+        <f t="shared" si="0"/>
         <v>1.0033735904357854E-6</v>
       </c>
       <c r="P3">
@@ -2691,7 +2694,7 @@
         <v>40.204736946868088</v>
       </c>
       <c r="Q3" s="25">
-        <f>ABS(O3)/L3</f>
+        <f t="shared" si="1"/>
         <v>2.5899774743874463E-8</v>
       </c>
     </row>
@@ -2737,7 +2740,7 @@
         <v>35.015823189882809</v>
       </c>
       <c r="O4">
-        <f>L4-N4</f>
+        <f t="shared" si="0"/>
         <v>6.8101171919465742E-6</v>
       </c>
       <c r="P4">
@@ -2745,7 +2748,7 @@
         <v>6.8430402635449381</v>
       </c>
       <c r="Q4" s="25">
-        <f>ABS(O4)/L4</f>
+        <f t="shared" si="1"/>
         <v>1.9448681330548423E-7</v>
       </c>
     </row>
@@ -2791,7 +2794,7 @@
         <v>38.855958684175874</v>
       </c>
       <c r="O5">
-        <f>L5-N5</f>
+        <f t="shared" si="0"/>
         <v>-8.684175874407174E-6</v>
       </c>
       <c r="P5">
@@ -2799,7 +2802,7 @@
         <v>41.680459434258815</v>
       </c>
       <c r="Q5" s="25">
-        <f>ABS(O5)/L5</f>
+        <f t="shared" si="1"/>
         <v>2.2349668131668827E-7</v>
       </c>
     </row>
@@ -2845,7 +2848,7 @@
         <v>38.52621298616311</v>
       </c>
       <c r="O6">
-        <f>L6-N6</f>
+        <f t="shared" si="0"/>
         <v>-2.9861631105632114E-6</v>
       </c>
       <c r="P6">
@@ -2853,7 +2856,7 @@
         <v>37.531558287554184</v>
       </c>
       <c r="Q6" s="25">
-        <f>ABS(O6)/L6</f>
+        <f t="shared" si="1"/>
         <v>7.7509911059593233E-8</v>
       </c>
     </row>
@@ -2899,7 +2902,7 @@
         <v>45.30356185119107</v>
       </c>
       <c r="O7">
-        <f>L7-N7</f>
+        <f t="shared" si="0"/>
         <v>8.1488089307413247E-6</v>
       </c>
       <c r="P7">
@@ -2907,7 +2910,7 @@
         <v>166.50445529184967</v>
       </c>
       <c r="Q7" s="25">
-        <f>ABS(O7)/L7</f>
+        <f t="shared" si="1"/>
         <v>1.7987123157714337E-7</v>
       </c>
     </row>
@@ -2953,7 +2956,7 @@
         <v>9.189302470419408</v>
       </c>
       <c r="O8">
-        <f>L8-N8</f>
+        <f t="shared" si="0"/>
         <v>4.5295805914946641E-6</v>
       </c>
       <c r="P8">
@@ -2961,7 +2964,7 @@
         <v>538.73206662757502</v>
       </c>
       <c r="Q8" s="25">
-        <f>ABS(O8)/L8</f>
+        <f t="shared" si="1"/>
         <v>4.9291862721472517E-7</v>
       </c>
     </row>
@@ -3007,7 +3010,7 @@
         <v>19.326641046455386</v>
       </c>
       <c r="O9">
-        <f>L9-N9</f>
+        <f t="shared" si="0"/>
         <v>-1.0464553845679347E-6</v>
       </c>
       <c r="P9">
@@ -3015,7 +3018,7 @@
         <v>170.91037441399396</v>
       </c>
       <c r="Q9" s="25">
-        <f>ABS(O9)/L9</f>
+        <f t="shared" si="1"/>
         <v>5.414574828153961E-8</v>
       </c>
     </row>
@@ -3061,7 +3064,7 @@
         <v>5.2532796663087629</v>
       </c>
       <c r="O10">
-        <f>L10-N10</f>
+        <f t="shared" si="0"/>
         <v>-6.6630876283113594E-7</v>
       </c>
       <c r="P10">
@@ -3069,7 +3072,7 @@
         <v>736.93954541532764</v>
       </c>
       <c r="Q10" s="25">
-        <f>ABS(O10)/L10</f>
+        <f t="shared" si="1"/>
         <v>1.2683673622343986E-7</v>
       </c>
     </row>
@@ -3115,7 +3118,7 @@
         <v>48.186951948272039</v>
       </c>
       <c r="O11">
-        <f>L11-N11</f>
+        <f t="shared" si="0"/>
         <v>-1.1948272039319363E-5</v>
       </c>
       <c r="P11">
@@ -3123,7 +3126,7 @@
         <v>249.23033322231737</v>
       </c>
       <c r="Q11" s="25">
-        <f>ABS(O11)/L11</f>
+        <f t="shared" si="1"/>
         <v>2.4795664633029951E-7</v>
       </c>
     </row>
@@ -3169,7 +3172,7 @@
         <v>27.136089644373062</v>
       </c>
       <c r="O12">
-        <f>L12-N12</f>
+        <f t="shared" si="0"/>
         <v>3.5562693767587916E-7</v>
       </c>
       <c r="P12">
@@ -3177,7 +3180,7 @@
         <v>27.707795323671011</v>
       </c>
       <c r="Q12" s="25">
-        <f>ABS(O12)/L12</f>
+        <f t="shared" si="1"/>
         <v>1.3105312433584912E-8</v>
       </c>
     </row>
@@ -3223,7 +3226,7 @@
         <v>50.595179579233545</v>
       </c>
       <c r="O13">
-        <f>L13-N13</f>
+        <f t="shared" si="0"/>
         <v>1.0420766457741593E-5</v>
       </c>
       <c r="P13">
@@ -3231,7 +3234,7 @@
         <v>331.06823387331747</v>
       </c>
       <c r="Q13" s="25">
-        <f>ABS(O13)/L13</f>
+        <f t="shared" si="1"/>
         <v>2.0596357989250741E-7</v>
       </c>
     </row>
@@ -3277,7 +3280,7 @@
         <v>45.222133144687149</v>
       </c>
       <c r="O14">
-        <f>L14-N14</f>
+        <f t="shared" si="0"/>
         <v>-3.1446871489038131E-6</v>
       </c>
       <c r="P14">
@@ -3285,7 +3288,7 @@
         <v>164.40933953694503</v>
       </c>
       <c r="Q14" s="25">
-        <f>ABS(O14)/L14</f>
+        <f t="shared" si="1"/>
         <v>6.9538678273310276E-8</v>
       </c>
     </row>
@@ -3331,7 +3334,7 @@
         <v>39.26274362009822</v>
       </c>
       <c r="O15">
-        <f>L15-N15</f>
+        <f t="shared" si="0"/>
         <v>6.379901776654151E-6</v>
       </c>
       <c r="P15">
@@ -3339,7 +3342,7 @@
         <v>47.098580256351084</v>
       </c>
       <c r="Q15" s="25">
-        <f>ABS(O15)/L15</f>
+        <f t="shared" si="1"/>
         <v>1.6249248401230559E-7</v>
       </c>
     </row>
@@ -3385,7 +3388,7 @@
         <v>14.653320024317317</v>
       </c>
       <c r="O16">
-        <f>L16-N16</f>
+        <f t="shared" si="0"/>
         <v>-2.431731616070465E-8</v>
       </c>
       <c r="P16">
@@ -3393,7 +3396,7 @@
         <v>314.94143751638779</v>
       </c>
       <c r="Q16" s="25">
-        <f>ABS(O16)/L16</f>
+        <f t="shared" si="1"/>
         <v>1.659508982312858E-9</v>
       </c>
     </row>
@@ -3439,7 +3442,7 @@
         <v>44.948480407189621</v>
       </c>
       <c r="O17">
-        <f>L17-N17</f>
+        <f t="shared" si="0"/>
         <v>-4.0718961713537283E-7</v>
       </c>
       <c r="P17">
@@ -3447,7 +3450,7 @@
         <v>157.46662255874512</v>
       </c>
       <c r="Q17" s="25">
-        <f>ABS(O17)/L17</f>
+        <f t="shared" si="1"/>
         <v>9.0590297410584925E-9</v>
       </c>
     </row>
@@ -3493,7 +3496,7 @@
         <v>32.25681720066104</v>
       </c>
       <c r="O18">
-        <f>L18-N18</f>
+        <f t="shared" si="0"/>
         <v>2.7993389579705763E-6</v>
       </c>
       <c r="P18">
@@ -3501,7 +3504,7 @@
         <v>2.047459400336608E-2</v>
       </c>
       <c r="Q18" s="25">
-        <f>ABS(O18)/L18</f>
+        <f t="shared" si="1"/>
         <v>8.6782855779663845E-8</v>
       </c>
     </row>
@@ -3547,7 +3550,7 @@
         <v>37.781020410530871</v>
       </c>
       <c r="O19">
-        <f>L19-N19</f>
+        <f t="shared" si="0"/>
         <v>-4.1053087329601112E-7</v>
       </c>
       <c r="P19">
@@ -3555,7 +3558,7 @@
         <v>28.956350627141862</v>
       </c>
       <c r="Q19" s="25">
-        <f>ABS(O19)/L19</f>
+        <f t="shared" si="1"/>
         <v>1.0866061141176473E-8</v>
       </c>
     </row>
@@ -3601,7 +3604,7 @@
         <v>21.168820559425473</v>
       </c>
       <c r="O20">
-        <f>L20-N20</f>
+        <f t="shared" si="0"/>
         <v>-5.5942547305676271E-7</v>
       </c>
       <c r="P20">
@@ -3609,7 +3612,7 @@
         <v>126.13737049308017</v>
       </c>
       <c r="Q20" s="25">
-        <f>ABS(O20)/L20</f>
+        <f t="shared" si="1"/>
         <v>2.6426861443234091E-8</v>
       </c>
     </row>
@@ -3655,7 +3658,7 @@
         <v>25.635152711607429</v>
       </c>
       <c r="O21">
-        <f>L21-N21</f>
+        <f t="shared" si="0"/>
         <v>-2.7116074292621306E-6</v>
       </c>
       <c r="P21">
@@ -3663,7 +3666,7 @@
         <v>45.761970572474077</v>
       </c>
       <c r="Q21" s="25">
-        <f>ABS(O21)/L21</f>
+        <f t="shared" si="1"/>
         <v>1.0577692852439446E-7</v>
       </c>
     </row>
@@ -3709,7 +3712,7 @@
         <v>40.422562462533605</v>
       </c>
       <c r="O22">
-        <f>L22-N22</f>
+        <f t="shared" si="0"/>
         <v>7.537466395035608E-6</v>
       </c>
       <c r="P22">
@@ -3717,7 +3720,7 @@
         <v>64.363082115388067</v>
       </c>
       <c r="Q22" s="25">
-        <f>ABS(O22)/L22</f>
+        <f t="shared" si="1"/>
         <v>1.8646677821414146E-7</v>
       </c>
     </row>
@@ -3763,7 +3766,7 @@
         <v>15.246817161811412</v>
       </c>
       <c r="O23">
-        <f>L23-N23</f>
+        <f t="shared" si="0"/>
         <v>2.838188587261925E-6</v>
       </c>
       <c r="P23">
@@ -3771,7 +3774,7 @@
         <v>294.22847807554166</v>
       </c>
       <c r="Q23" s="25">
-        <f>ABS(O23)/L23</f>
+        <f t="shared" si="1"/>
         <v>1.8614954379089705E-7</v>
       </c>
     </row>
@@ -3817,7 +3820,7 @@
         <v>28.678232870435906</v>
       </c>
       <c r="O24">
-        <f>L24-N24</f>
+        <f t="shared" si="0"/>
         <v>-2.8704359067432961E-6</v>
       </c>
       <c r="P24">
@@ -3825,7 +3828,7 @@
         <v>13.850898014437181</v>
       </c>
       <c r="Q24" s="25">
-        <f>ABS(O24)/L24</f>
+        <f t="shared" si="1"/>
         <v>1.0009111115795138E-7</v>
       </c>
     </row>
@@ -3871,7 +3874,7 @@
         <v>48.141080049067014</v>
       </c>
       <c r="O25">
-        <f>L25-N25</f>
+        <f t="shared" si="0"/>
         <v>-4.9067011786974035E-8</v>
       </c>
       <c r="P25">
@@ -3879,7 +3882,7 @@
         <v>247.78444992092975</v>
       </c>
       <c r="Q25" s="25">
-        <f>ABS(O25)/L25</f>
+        <f t="shared" si="1"/>
         <v>1.0192337144695141E-9</v>
       </c>
     </row>
@@ -3925,7 +3928,7 @@
         <v>40.147488385176963</v>
       </c>
       <c r="O26">
-        <f>L26-N26</f>
+        <f t="shared" si="0"/>
         <v>-8.3851769616671845E-6</v>
       </c>
       <c r="P26">
@@ -3933,7 +3936,7 @@
         <v>60.02484924843732</v>
       </c>
       <c r="Q26" s="25">
-        <f>ABS(O26)/L26</f>
+        <f t="shared" si="1"/>
         <v>2.0885935958289746E-7</v>
       </c>
     </row>
@@ -3979,7 +3982,7 @@
         <v>26.668283706736183</v>
       </c>
       <c r="O27">
-        <f>L27-N27</f>
+        <f t="shared" si="0"/>
         <v>-3.7067361837728185E-6</v>
       </c>
       <c r="P27">
@@ -3987,7 +3990,7 @@
         <v>32.851576284375625</v>
       </c>
       <c r="Q27" s="25">
-        <f>ABS(O27)/L27</f>
+        <f t="shared" si="1"/>
         <v>1.3899419774251727E-7</v>
       </c>
     </row>

</xml_diff>